<commit_message>
adding strain names run 1755 to 2641
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_0673.xlsx
+++ b/bioSample/bioSample_0673.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0076637B-47C5-524B-A9D9-21D1A0CB20B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA07957-E476-EB45-A96A-A0349C81B094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="22">
   <si>
     <t>harvestDate</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>90minuteInduction</t>
-  </si>
-  <si>
-    <t>KN99alpha</t>
   </si>
   <si>
     <t>CNAG_00000</t>
@@ -474,7 +471,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E13"/>
+      <selection activeCell="E12" sqref="E12:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -525,13 +522,13 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2">
         <v>90</v>
@@ -554,13 +551,13 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3">
         <v>90</v>
@@ -583,13 +580,13 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4">
         <v>90</v>
@@ -612,13 +609,13 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5">
         <v>90</v>
@@ -641,13 +638,13 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
         <v>15</v>
       </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6">
         <v>90</v>
@@ -670,13 +667,13 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
         <v>15</v>
       </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7">
         <v>90</v>
@@ -699,13 +696,13 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
         <v>17</v>
       </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8">
         <v>90</v>
@@ -728,13 +725,13 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9">
         <v>90</v>
@@ -757,13 +754,13 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10">
         <v>90</v>
@@ -774,7 +771,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -786,13 +783,13 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
         <v>12</v>
       </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11">
         <v>90</v>
@@ -803,7 +800,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -815,13 +812,13 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
         <v>12</v>
       </c>
-      <c r="F12" t="s">
-        <v>13</v>
-      </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H12">
         <v>90</v>
@@ -832,7 +829,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -844,13 +841,13 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
         <v>12</v>
       </c>
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H13">
         <v>90</v>
@@ -861,7 +858,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -873,13 +870,13 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
         <v>20</v>
       </c>
-      <c r="F14" t="s">
-        <v>21</v>
-      </c>
       <c r="G14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14">
         <v>90</v>
@@ -890,7 +887,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -902,13 +899,13 @@
         <v>11</v>
       </c>
       <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
         <v>20</v>
       </c>
-      <c r="F15" t="s">
-        <v>21</v>
-      </c>
       <c r="G15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H15">
         <v>90</v>
@@ -919,7 +916,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -931,13 +928,13 @@
         <v>11</v>
       </c>
       <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
         <v>20</v>
       </c>
-      <c r="F16" t="s">
-        <v>21</v>
-      </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16">
         <v>90</v>

</xml_diff>